<commit_message>
Use DIV_1 instead of DIV_8; DIV_1 gave more comprehendable results.
</commit_message>
<xml_diff>
--- a/uC/MSP430/QKNLatency/Result.xlsx
+++ b/uC/MSP430/QKNLatency/Result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>TBCCR1</t>
   </si>
@@ -62,6 +62,27 @@
   <si>
     <t>Delay</t>
   </si>
+  <si>
+    <t>Pulsewidth [us]</t>
+  </si>
+  <si>
+    <t>Prediction [us]</t>
+  </si>
+  <si>
+    <t>Error [us]</t>
+  </si>
+  <si>
+    <t>TBCCR1 [clk]</t>
+  </si>
+  <si>
+    <t>t1 [clk]</t>
+  </si>
+  <si>
+    <t>t3 [clk]</t>
+  </si>
+  <si>
+    <t>Latency  [clk]</t>
+  </si>
 </sst>
 </file>
 
@@ -96,13 +117,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -160,10 +203,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$12:$A$24</c:f>
+              <c:f>Sheet1!$A$12:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -171,36 +214,33 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>200</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>400</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>1600</c:v>
                 </c:pt>
               </c:numCache>
@@ -208,47 +248,44 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$12:$F$24</c:f>
+              <c:f>Sheet1!$F$12:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>-1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>99</c:v>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>199</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>400</c:v>
+                  <c:v>799</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>799</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>1599</c:v>
                 </c:pt>
               </c:numCache>
@@ -264,8 +301,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="39710720"/>
-        <c:axId val="39708928"/>
+        <c:axId val="107543552"/>
+        <c:axId val="108135552"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -291,10 +328,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$12:$A$24</c:f>
+              <c:f>Sheet1!$A$12:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -302,36 +339,33 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>200</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>400</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>1600</c:v>
                 </c:pt>
               </c:numCache>
@@ -339,36 +373,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$12:$G$24</c:f>
+              <c:f>Sheet1!$G$12:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>36</c:v>
@@ -377,9 +411,6 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
@@ -395,11 +426,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47357952"/>
-        <c:axId val="110286336"/>
+        <c:axId val="108147840"/>
+        <c:axId val="108137472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39710720"/>
+        <c:axId val="107543552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,12 +459,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39708928"/>
+        <c:crossAx val="108135552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39708928"/>
+        <c:axId val="108135552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,12 +493,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39710720"/>
+        <c:crossAx val="107543552"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110286336"/>
+        <c:axId val="108137472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -498,12 +529,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47357952"/>
+        <c:crossAx val="108147840"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47357952"/>
+        <c:axId val="108147840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,7 +544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110286336"/>
+        <c:crossAx val="108137472"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -549,20 +580,374 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pulsewidth [us]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$26:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7820</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7880</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$26:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>504.875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>967.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>979.875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>982.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>992.375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Error [us]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$26:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7820</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7880</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$26:$H$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="146391424"/>
+        <c:axId val="108283392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="146391424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Timer B load value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108283392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="108283392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pulsewidth [usec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146391424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.66181583323027027"/>
+          <c:y val="0.41289761027337946"/>
+          <c:w val="0.33818433467520742"/>
+          <c:h val="0.18440195809597529"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>366712</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -576,6 +961,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>119061</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -599,19 +1014,46 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A11:G24" totalsRowShown="0">
-  <autoFilter ref="A11:G24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A11:G23" totalsRowShown="0">
+  <autoFilter ref="A11:G23"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Delay"/>
     <tableColumn id="2" name="DIV"/>
     <tableColumn id="3" name="t1"/>
     <tableColumn id="4" name="t2"/>
     <tableColumn id="5" name="t3"/>
-    <tableColumn id="6" name="ISR latency" dataDxfId="1">
+    <tableColumn id="6" name="ISR latency" dataDxfId="7">
       <calculatedColumnFormula>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="QK latency" dataDxfId="0">
+    <tableColumn id="7" name="QK latency" dataDxfId="6">
       <calculatedColumnFormula>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A25:H37" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A25:H37"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="TBCCR1 [clk]" dataDxfId="5">
+      <calculatedColumnFormula>8000 - 300</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="DIV"/>
+    <tableColumn id="3" name="t1 [clk]"/>
+    <tableColumn id="5" name="t3 [clk]"/>
+    <tableColumn id="7" name="Latency  [clk]" dataDxfId="4">
+      <calculatedColumnFormula>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Pulsewidth [us]" dataDxfId="3">
+      <calculatedColumnFormula>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Prediction [us]" dataDxfId="2">
+      <calculatedColumnFormula xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Error [us]" dataDxfId="1">
+      <calculatedColumnFormula>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -905,19 +1347,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -941,7 +1388,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -961,10 +1408,10 @@
         <v>5</v>
       </c>
       <c r="H2">
-        <v>16000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -985,10 +1432,10 @@
       </c>
       <c r="H3">
         <f>H2/8</f>
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1011,7 +1458,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -1032,10 +1479,10 @@
       </c>
       <c r="H5">
         <f>H3/H4</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -1056,10 +1503,10 @@
       </c>
       <c r="H6">
         <f>H1/H3</f>
-        <v>3.2767999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6.5535999999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -1082,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50</v>
       </c>
@@ -1099,7 +1546,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>100</v>
       </c>
@@ -1116,7 +1563,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1138,8 +1585,12 @@
       <c r="G11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f>G12*B12</f>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1150,21 +1601,21 @@
         <v>21</v>
       </c>
       <c r="D12">
-        <v>21</v>
+        <v>770</v>
       </c>
       <c r="E12">
-        <v>58</v>
+        <v>808</v>
       </c>
       <c r="F12">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>-1</v>
+        <v>748</v>
       </c>
       <c r="G12">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1175,46 +1626,46 @@
         <v>21</v>
       </c>
       <c r="D13">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>59</v>
       </c>
       <c r="F13">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G13">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>8</v>
       </c>
       <c r="C14">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D14">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E14">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F14">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G14">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1222,13 +1673,13 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D15">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E15">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="F15">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
@@ -1236,137 +1687,137 @@
       </c>
       <c r="G15">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E16">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="F16">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G16">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>8</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D17">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="E17">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="F17">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G17">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D18">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="E18">
-        <v>83</v>
+        <v>157</v>
       </c>
       <c r="F18">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G18">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B19">
         <v>8</v>
       </c>
       <c r="C19">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="D19">
-        <v>72</v>
+        <v>221</v>
       </c>
       <c r="E19">
-        <v>109</v>
+        <v>258</v>
       </c>
       <c r="F19">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="G19">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B20">
         <v>8</v>
       </c>
       <c r="C20">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20">
-        <v>121</v>
+        <v>220</v>
       </c>
       <c r="E20">
-        <v>159</v>
+        <v>257</v>
       </c>
       <c r="F20">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>99</v>
+        <v>199</v>
       </c>
       <c r="G20">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="B21">
         <v>8</v>
@@ -1375,48 +1826,48 @@
         <v>20</v>
       </c>
       <c r="D21">
-        <v>220</v>
+        <v>421</v>
       </c>
       <c r="E21">
-        <v>257</v>
+        <v>458</v>
       </c>
       <c r="F21">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>199</v>
+        <v>400</v>
       </c>
       <c r="G21">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="B22">
         <v>8</v>
       </c>
       <c r="C22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22">
-        <v>421</v>
+        <v>821</v>
       </c>
       <c r="E22">
-        <v>458</v>
+        <v>858</v>
       </c>
       <c r="F22">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>400</v>
+        <v>799</v>
       </c>
       <c r="G22">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -1425,51 +1876,414 @@
         <v>21</v>
       </c>
       <c r="D23">
-        <v>821</v>
+        <v>1621</v>
       </c>
       <c r="E23">
-        <v>858</v>
+        <v>1659</v>
       </c>
       <c r="F23">
         <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>799</v>
+        <v>1599</v>
       </c>
       <c r="G23">
         <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1600</v>
-      </c>
-      <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D24">
-        <v>1621</v>
-      </c>
-      <c r="E24">
-        <v>1659</v>
-      </c>
-      <c r="F24">
-        <f>Table13[[#This Row],[t2]] - Table13[[#This Row],[t1]] - $H$7</f>
-        <v>1599</v>
-      </c>
-      <c r="G24">
-        <f>Table13[[#This Row],[t3]]-Table13[[#This Row],[t2]]-$H$7</f>
-        <v>37</v>
+      <c r="F25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>96</v>
+      </c>
+      <c r="E26">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>80</v>
+      </c>
+      <c r="F26">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>10</v>
+      </c>
+      <c r="H26" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>106</v>
+      </c>
+      <c r="E27">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>90</v>
+      </c>
+      <c r="F27">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>11.25</v>
+      </c>
+      <c r="G27">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>11.25</v>
+      </c>
+      <c r="H27" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>70</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>127</v>
+      </c>
+      <c r="E28">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>110</v>
+      </c>
+      <c r="F28">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>13.75</v>
+      </c>
+      <c r="G28">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>13.75</v>
+      </c>
+      <c r="H28" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>75</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>131</v>
+      </c>
+      <c r="E29">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>115</v>
+      </c>
+      <c r="F29">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>14.375</v>
+      </c>
+      <c r="G29">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>14.375</v>
+      </c>
+      <c r="H29" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>80</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>17</v>
+      </c>
+      <c r="D30">
+        <v>137</v>
+      </c>
+      <c r="E30">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>120</v>
+      </c>
+      <c r="F30">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>15</v>
+      </c>
+      <c r="G30">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>15</v>
+      </c>
+      <c r="H30" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>800</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>17</v>
+      </c>
+      <c r="D31">
+        <v>857</v>
+      </c>
+      <c r="E31">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>840</v>
+      </c>
+      <c r="F31">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>105</v>
+      </c>
+      <c r="G31">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>105</v>
+      </c>
+      <c r="H31" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>4000</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>16</v>
+      </c>
+      <c r="D32">
+        <v>4055</v>
+      </c>
+      <c r="E32">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>4039</v>
+      </c>
+      <c r="F32">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>504.875</v>
+      </c>
+      <c r="G32">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>505</v>
+      </c>
+      <c r="H32" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7700</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>17</v>
+      </c>
+      <c r="D33">
+        <v>7757</v>
+      </c>
+      <c r="E33">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>7740</v>
+      </c>
+      <c r="F33">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>967.5</v>
+      </c>
+      <c r="G33">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>967.5</v>
+      </c>
+      <c r="H33" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>7800</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>17</v>
+      </c>
+      <c r="D34">
+        <v>7856</v>
+      </c>
+      <c r="E34" s="1">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>7839</v>
+      </c>
+      <c r="F34">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>979.875</v>
+      </c>
+      <c r="G34">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>980</v>
+      </c>
+      <c r="H34" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>7820</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>17</v>
+      </c>
+      <c r="D35">
+        <v>7876</v>
+      </c>
+      <c r="E35" s="1">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>7859</v>
+      </c>
+      <c r="F35" s="1">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>982.375</v>
+      </c>
+      <c r="G35">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>982.5</v>
+      </c>
+      <c r="H35" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>7880</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>17</v>
+      </c>
+      <c r="D36">
+        <v>7937</v>
+      </c>
+      <c r="E36" s="1">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>7920</v>
+      </c>
+      <c r="F36" s="1">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>990</v>
+      </c>
+      <c r="G36">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>990</v>
+      </c>
+      <c r="H36" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>7900</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>17</v>
+      </c>
+      <c r="D37">
+        <v>7956</v>
+      </c>
+      <c r="E37" s="1">
+        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
+        <v>7939</v>
+      </c>
+      <c r="F37">
+        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
+        <v>992.375</v>
+      </c>
+      <c r="G37">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+        <v>992.5</v>
+      </c>
+      <c r="H37" s="1">
+        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Talked to ST L6470 from MSP430 Launchpad for the first time
</commit_message>
<xml_diff>
--- a/uC/MSP430/QKNLatency/Result.xlsx
+++ b/uC/MSP430/QKNLatency/Result.xlsx
@@ -129,7 +129,7 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -144,7 +144,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -301,8 +301,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107543552"/>
-        <c:axId val="108135552"/>
+        <c:axId val="110620032"/>
+        <c:axId val="110888448"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -426,11 +426,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108147840"/>
-        <c:axId val="108137472"/>
+        <c:axId val="110892544"/>
+        <c:axId val="110890368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107543552"/>
+        <c:axId val="110620032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -459,12 +459,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108135552"/>
+        <c:crossAx val="110888448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108135552"/>
+        <c:axId val="110888448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -493,12 +493,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107543552"/>
+        <c:crossAx val="110620032"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108137472"/>
+        <c:axId val="110890368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -529,12 +529,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108147840"/>
+        <c:crossAx val="110892544"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108147840"/>
+        <c:axId val="110892544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,7 +544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108137472"/>
+        <c:crossAx val="110890368"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -621,10 +621,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$37</c:f>
+              <c:f>Sheet1!$A$27:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -632,79 +632,37 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7820</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7880</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7900</c:v>
+                  <c:v>7872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$26:$F$37</c:f>
+              <c:f>Sheet1!$F$27:$F$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.25</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.75</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.375</c:v>
+                  <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>504.875</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>967.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>979.875</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>982.375</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>990</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>992.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -732,10 +690,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$26:$A$37</c:f>
+              <c:f>Sheet1!$A$27:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -743,44 +701,23 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7700</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7820</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7880</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7900</c:v>
+                  <c:v>7872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$26:$H$37</c:f>
+              <c:f>Sheet1!$H$27:$H$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -795,27 +732,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -830,11 +746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="146391424"/>
-        <c:axId val="108283392"/>
+        <c:axId val="110925696"/>
+        <c:axId val="110936064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="146391424"/>
+        <c:axId val="110925696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,12 +779,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108283392"/>
+        <c:crossAx val="110936064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108283392"/>
+        <c:axId val="110936064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +814,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146391424"/>
+        <c:crossAx val="110925696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -970,13 +886,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>119061</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1034,23 +950,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A25:H37" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A25:H37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A25:H31" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A25:H31"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="TBCCR1 [clk]" dataDxfId="5">
+    <tableColumn id="1" name="TBCCR1 [clk]" dataDxfId="4">
       <calculatedColumnFormula>8000 - 300</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="DIV"/>
     <tableColumn id="3" name="t1 [clk]"/>
     <tableColumn id="5" name="t3 [clk]"/>
-    <tableColumn id="7" name="Latency  [clk]" dataDxfId="4">
+    <tableColumn id="7" name="Latency  [clk]" dataDxfId="3">
       <calculatedColumnFormula>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Pulsewidth [us]" dataDxfId="3">
+    <tableColumn id="4" name="Pulsewidth [us]" dataDxfId="2">
       <calculatedColumnFormula>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Prediction [us]" dataDxfId="2">
-      <calculatedColumnFormula xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</calculatedColumnFormula>
+    <tableColumn id="6" name="Prediction [us]" dataDxfId="0">
+      <calculatedColumnFormula xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 48)/$H$2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Error [us]" dataDxfId="1">
       <calculatedColumnFormula>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</calculatedColumnFormula>
@@ -1347,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,28 +1833,28 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>40</v>
+      <c r="A26" s="1">
+        <v>32</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D26">
-        <v>96</v>
-      </c>
-      <c r="E26">
+        <v>130</v>
+      </c>
+      <c r="E26" s="1">
         <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
         <v>80</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
         <v>10</v>
       </c>
-      <c r="G26">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
+      <c r="G26" s="1">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 48)/$H$2</f>
         <v>10</v>
       </c>
       <c r="H26" s="1">
@@ -1947,29 +1863,29 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>50</v>
+      <c r="A27" s="1">
+        <v>40</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="D27">
-        <v>106</v>
-      </c>
-      <c r="E27">
+        <v>146</v>
+      </c>
+      <c r="E27" s="1">
         <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>90</v>
-      </c>
-      <c r="F27">
+        <v>88</v>
+      </c>
+      <c r="F27" s="1">
         <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>11.25</v>
-      </c>
-      <c r="G27">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>11.25</v>
+        <v>11</v>
+      </c>
+      <c r="G27" s="1">
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 48)/$H$2</f>
+        <v>11</v>
       </c>
       <c r="H27" s="1">
         <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
@@ -1978,28 +1894,28 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="D28">
-        <v>127</v>
+        <v>167</v>
       </c>
       <c r="E28">
         <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F28">
         <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>13.75</v>
+        <v>12.25</v>
       </c>
       <c r="G28">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>13.75</v>
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 48)/$H$2</f>
+        <v>12.25</v>
       </c>
       <c r="H28" s="1">
         <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
@@ -2008,28 +1924,28 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>75</v>
+        <v>800</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>16</v>
+        <v>818</v>
       </c>
       <c r="D29">
-        <v>131</v>
+        <v>1666</v>
       </c>
       <c r="E29">
         <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>115</v>
+        <v>848</v>
       </c>
       <c r="F29">
         <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>14.375</v>
+        <v>106</v>
       </c>
       <c r="G29">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>14.375</v>
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 48)/$H$2</f>
+        <v>106</v>
       </c>
       <c r="H29" s="1">
         <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
@@ -2038,28 +1954,28 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>80</v>
+        <v>4000</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30">
-        <v>17</v>
+        <v>9969</v>
       </c>
       <c r="D30">
-        <v>137</v>
+        <v>14017</v>
       </c>
       <c r="E30">
         <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>120</v>
+        <v>4048</v>
       </c>
       <c r="F30">
         <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>15</v>
+        <v>506</v>
       </c>
       <c r="G30">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>15</v>
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 48)/$H$2</f>
+        <v>506</v>
       </c>
       <c r="H30" s="1">
         <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
@@ -2067,213 +1983,33 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>800</v>
+      <c r="A31" s="1">
+        <v>7872</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>17</v>
+        <v>7891</v>
       </c>
       <c r="D31">
-        <v>857</v>
-      </c>
-      <c r="E31">
+        <v>15811</v>
+      </c>
+      <c r="E31" s="1">
         <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>840</v>
-      </c>
-      <c r="F31">
+        <v>7920</v>
+      </c>
+      <c r="F31" s="1">
         <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>105</v>
+        <v>990</v>
       </c>
       <c r="G31">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>105</v>
+        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 48)/$H$2</f>
+        <v>990</v>
       </c>
       <c r="H31" s="1">
         <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>4000</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>16</v>
-      </c>
-      <c r="D32">
-        <v>4055</v>
-      </c>
-      <c r="E32">
-        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>4039</v>
-      </c>
-      <c r="F32">
-        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>504.875</v>
-      </c>
-      <c r="G32">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>505</v>
-      </c>
-      <c r="H32" s="1">
-        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>7700</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>17</v>
-      </c>
-      <c r="D33">
-        <v>7757</v>
-      </c>
-      <c r="E33">
-        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>7740</v>
-      </c>
-      <c r="F33">
-        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>967.5</v>
-      </c>
-      <c r="G33">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>967.5</v>
-      </c>
-      <c r="H33" s="1">
-        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>7800</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>17</v>
-      </c>
-      <c r="D34">
-        <v>7856</v>
-      </c>
-      <c r="E34" s="1">
-        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>7839</v>
-      </c>
-      <c r="F34">
-        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>979.875</v>
-      </c>
-      <c r="G34">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>980</v>
-      </c>
-      <c r="H34" s="1">
-        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>7820</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>17</v>
-      </c>
-      <c r="D35">
-        <v>7876</v>
-      </c>
-      <c r="E35" s="1">
-        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>7859</v>
-      </c>
-      <c r="F35" s="1">
-        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>982.375</v>
-      </c>
-      <c r="G35">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>982.5</v>
-      </c>
-      <c r="H35" s="1">
-        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>7880</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>17</v>
-      </c>
-      <c r="D36">
-        <v>7937</v>
-      </c>
-      <c r="E36" s="1">
-        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>7920</v>
-      </c>
-      <c r="F36" s="1">
-        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>990</v>
-      </c>
-      <c r="G36">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>990</v>
-      </c>
-      <c r="H36" s="1">
-        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>7900</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>17</v>
-      </c>
-      <c r="D37">
-        <v>7956</v>
-      </c>
-      <c r="E37" s="1">
-        <f>Table134[[#This Row],[t3 '[clk']]]-Table134[[#This Row],[t1 '[clk']]]</f>
-        <v>7939</v>
-      </c>
-      <c r="F37">
-        <f>1000000 * Table134[[#This Row],[Latency  '[clk']]]/$H$2</f>
-        <v>992.375</v>
-      </c>
-      <c r="G37">
-        <f xml:space="preserve"> 1000000* (Table134[[#This Row],[TBCCR1 '[clk']]] + 40)/$H$2</f>
-        <v>992.5</v>
-      </c>
-      <c r="H37" s="1">
-        <f>Table134[[#This Row],[Prediction '[us']]]-Table134[[#This Row],[Pulsewidth '[us']]]</f>
-        <v>0.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>